<commit_message>
Uren Registratie 04-02-2016 & Bug Report fix
</commit_message>
<xml_diff>
--- a/Algemeen/Bug Report.xlsx
+++ b/Algemeen/Bug Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="54">
   <si>
     <t>Bug nr.</t>
   </si>
@@ -115,9 +115,6 @@
     <t>niet.</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
     <t>Fahrettin</t>
   </si>
   <si>
@@ -136,32 +133,56 @@
     <t xml:space="preserve">Paraaf: </t>
   </si>
   <si>
-    <t>Voorbeeld</t>
-  </si>
-  <si>
-    <t>pre-Alpha</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
-    <t>Player</t>
-  </si>
-  <si>
     <t>Mack</t>
   </si>
   <si>
-    <t>Player kan niet goed poepen</t>
-  </si>
-  <si>
-    <t>Zit op de WC zonder Bril</t>
+    <t>Coding Error</t>
+  </si>
+  <si>
+    <t>Expected Result:</t>
+  </si>
+  <si>
+    <t>Actual Result:</t>
+  </si>
+  <si>
+    <t>Het is onmogelijk om jumps in de game te</t>
+  </si>
+  <si>
+    <t>halen, ondanks dat de springafstanden kloppen</t>
+  </si>
+  <si>
+    <t>volgens plan.</t>
+  </si>
+  <si>
+    <t>Dev-Fase-1</t>
+  </si>
+  <si>
+    <t>Dejump halen</t>
+  </si>
+  <si>
+    <t>De speler haalt de jump net niet en valt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3: Probeer over het gat heen te springen met spatie en de </t>
+  </si>
+  <si>
+    <t>right arrow.</t>
+  </si>
+  <si>
+    <t>1: Laad level 1.</t>
+  </si>
+  <si>
+    <t>2: Ga op de uiterste rand staan voor je valt.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +205,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -214,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -314,13 +342,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -334,24 +402,38 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Goed" xfId="2" builtinId="26"/>
@@ -658,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z62"/>
+  <dimension ref="A1:Z65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+      <selection activeCell="L68" sqref="L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +849,7 @@
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="5"/>
@@ -884,12 +966,12 @@
     <row r="10" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="11"/>
       <c r="O10" s="3"/>
       <c r="P10" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q10" s="9"/>
     </row>
@@ -955,7 +1037,7 @@
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1019,7 +1101,7 @@
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="11"/>
     </row>
@@ -1085,7 +1167,7 @@
       </c>
       <c r="K29" s="6"/>
       <c r="L29" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1148,7 +1230,7 @@
     <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="11"/>
     </row>
@@ -1214,7 +1296,7 @@
       </c>
       <c r="K42" s="6"/>
       <c r="L42" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1284,163 +1366,246 @@
     <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C49" s="11"/>
     </row>
+    <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="2" t="s">
+      <c r="A53" s="19"/>
+      <c r="B53" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="23"/>
+      <c r="D53" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" s="23"/>
+      <c r="F53" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="23"/>
+      <c r="H53" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I53" s="23"/>
+      <c r="J53" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="K53" s="23"/>
+      <c r="L53" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="20"/>
+      <c r="B54" s="26">
+        <v>1</v>
+      </c>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27">
+        <v>1</v>
+      </c>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K54" s="27"/>
+      <c r="L54" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G54" s="4"/>
-      <c r="H54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I54" s="4"/>
-      <c r="J54" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="13"/>
-      <c r="B55" s="15">
-        <v>1</v>
-      </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E55" s="16"/>
-      <c r="F55" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G55" s="16"/>
-      <c r="H55" s="17" t="s">
+    </row>
+    <row r="55" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="19"/>
+      <c r="B55" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="23"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="23"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="9"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="19"/>
+      <c r="B56" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32"/>
+      <c r="L56" s="33"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="19"/>
+      <c r="B57" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="15"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="19"/>
+      <c r="B58" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="15"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="19"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="15"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
+      <c r="B60" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="I55" s="16"/>
-      <c r="J55" s="17" t="s">
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="15"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="19"/>
+      <c r="B61" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="15"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="19"/>
+      <c r="B62" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="K55" s="16"/>
-      <c r="L55" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
-      <c r="B56" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H56" s="9"/>
-      <c r="L56" s="3"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="C57" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="20"/>
-      <c r="H57" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="20"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="20"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="20"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="20"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="20"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="20"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="20"/>
-    </row>
-    <row r="61" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="6"/>
-    </row>
-    <row r="62" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3"/>
-      <c r="B62" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>44</v>
-      </c>
+      <c r="C62" s="22"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="15"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="19"/>
+      <c r="B63" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="15"/>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="19"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="17"/>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="19"/>
+      <c r="B65" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+      <c r="L65" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>